<commit_message>
2.1.5 Added more consistent handling to keys in the from_dict constructor. standardized model property names.
</commit_message>
<xml_diff>
--- a/samples/Tricuspid_Valve_Atresia/Tricuspid_Valve_Atresia_Fhir_Cohort_Import_Template.xlsx
+++ b/samples/Tricuspid_Valve_Atresia/Tricuspid_Valve_Atresia_Fhir_Cohort_Import_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mriley7/workspace/FHIRSheets/samples/Tricuspid_Valve_Atresia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135E0B5C-2C58-2648-BBC8-3DBCBC16DA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE6CA27-9BCA-9245-B233-C9516CC4ABD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{B7CAF98F-F4CF-4673-A736-BDE9BA8D985C}"/>
+    <workbookView xWindow="-34720" yWindow="120" windowWidth="30240" windowHeight="17820" activeTab="3" xr2:uid="{B7CAF98F-F4CF-4673-A736-BDE9BA8D985C}"/>
   </bookViews>
   <sheets>
     <sheet name="How To Use This Workbook" sheetId="6" r:id="rId1"/>
@@ -2884,7 +2884,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3209,7 +3209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1F7A94-D1C6-4537-A70E-D5B7DD1165E4}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -3568,9 +3568,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB4DC11-02AF-44A1-9E33-056BEEEC10B1}">
   <dimension ref="A1:DZ16"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="40" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="40" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AP11" sqref="AP11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7035,8 +7035,8 @@
   <dimension ref="A1:DQ16"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BJ1" sqref="BJ1:BL1048576"/>
+      <pane xSplit="1" topLeftCell="CE1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CI6" sqref="CI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>